<commit_message>
A9 Final Working Commit
</commit_message>
<xml_diff>
--- a/questions/Assignment9-ClientCommandTableForA9 .xlsx
+++ b/questions/Assignment9-ClientCommandTableForA9 .xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viswesh\SimplicityStudio\v5_workspace\ecen5823-assignment9-VisweshBaskaran\questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viswesh\Desktop\ecen5823-assignment9-VisweshBaskaran\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F83B27-0BE1-4FFF-B81C-D9CAEE9374F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D0BA6-AA67-498B-9BDC-FE0CDD443C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,9 +587,6 @@
     </r>
   </si>
   <si>
-    <t>DISCOVERY STATE MACHINE for A7</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">  sl_bt_scanner_stop() on </t>
     </r>
@@ -1158,6 +1155,9 @@
   </si>
   <si>
     <t>DISPLAY_ROW_CONNECTION, "Bonded" on server and client</t>
+  </si>
+  <si>
+    <t>DISCOVERY STATE MACHINE for A9</t>
   </si>
 </sst>
 </file>
@@ -1643,22 +1643,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>851646</xdr:colOff>
+      <xdr:colOff>974913</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>123265</xdr:rowOff>
+      <xdr:rowOff>212910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>672028</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>372218</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>408939</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22410</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F84C62DA-2C08-DB69-57C7-4AA7DFCA10FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A9CBA3-58DF-71D0-DBD6-358994FC3356}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,8 +1674,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15833911" y="694765"/>
-          <a:ext cx="9726382" cy="5325218"/>
+          <a:off x="20394707" y="784410"/>
+          <a:ext cx="15861850" cy="5614147"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1686,23 +1686,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2442882</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>56029</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>4951282</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>150828</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>31899</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>139623</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E5ED79-EABB-7DCB-7FCF-D99F4BEFAA8B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE89BFE0-954E-46AF-9E87-52CF3E5E03E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1718,7 +1718,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11530853" y="26333823"/>
+          <a:off x="20506765" y="8292353"/>
           <a:ext cx="7763958" cy="4801270"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2811,8 +2811,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2831,7 +2831,7 @@
     <row r="1" spans="1:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15"/>
       <c r="B1" s="44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
@@ -2846,7 +2846,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="H2" s="27" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="119.65" customHeight="1" x14ac:dyDescent="0.2">
@@ -2903,7 +2903,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2962,11 +2962,11 @@
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2974,11 +2974,11 @@
       <c r="A12" s="18"/>
       <c r="B12" s="18"/>
       <c r="C12" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2986,7 +2986,7 @@
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
       <c r="C13" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="7" t="s">
@@ -2998,7 +2998,7 @@
       <c r="A14" s="18"/>
       <c r="B14" s="18"/>
       <c r="C14" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
@@ -3010,7 +3010,7 @@
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
@@ -3028,7 +3028,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="18"/>
       <c r="C17" s="3"/>
@@ -3036,7 +3036,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="9" t="s">
         <v>28</v>
@@ -3048,11 +3048,11 @@
         <v>24</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="3"/>
@@ -3064,7 +3064,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18"/>
       <c r="B20" s="9" t="s">
         <v>27</v>
@@ -3076,11 +3076,14 @@
         <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="3"/>
@@ -3088,7 +3091,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="9" t="s">
         <v>14</v>
@@ -3100,7 +3103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="35"/>
       <c r="B23" s="39"/>
       <c r="C23" s="36"/>
@@ -3108,45 +3111,45 @@
       <c r="E23" s="40"/>
       <c r="F23" s="41"/>
     </row>
-    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="35"/>
       <c r="B24" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F24" s="36"/>
     </row>
-    <row r="25" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="42"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
       <c r="E25" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F25" s="36"/>
     </row>
-    <row r="26" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="42"/>
       <c r="B26" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="36"/>
       <c r="D26" s="36"/>
       <c r="E26" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F26" s="41" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="42"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
@@ -3154,21 +3157,21 @@
       <c r="E27" s="36"/>
       <c r="F27" s="36"/>
     </row>
-    <row r="28" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="42"/>
       <c r="B28" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
       <c r="F28" s="41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="42"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
@@ -3176,19 +3179,19 @@
       <c r="E29" s="36"/>
       <c r="F29" s="36"/>
     </row>
-    <row r="30" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="42"/>
       <c r="B30" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="36"/>
       <c r="D30" s="36"/>
       <c r="E30" s="36"/>
       <c r="F30" s="41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="42"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
@@ -3196,18 +3199,18 @@
       <c r="E31" s="36"/>
       <c r="F31" s="36"/>
     </row>
-    <row r="32" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="42"/>
       <c r="B32" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>
       <c r="F32" s="41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3236,7 +3239,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35" s="26" t="s">
         <v>17</v>
@@ -3260,7 +3263,7 @@
         <v>24</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F37" s="33" t="s">
         <v>44</v>
@@ -3274,7 +3277,7 @@
         <v>24</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -3286,7 +3289,7 @@
         <v>24</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -3298,7 +3301,7 @@
         <v>24</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -3310,7 +3313,7 @@
         <v>24</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -3320,7 +3323,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="6"/>
       <c r="E42" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F42" s="3"/>
     </row>
@@ -3339,7 +3342,7 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="25" t="s">
@@ -3361,7 +3364,7 @@
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="25" t="s">
@@ -3379,7 +3382,7 @@
     <row r="48" spans="1:6" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -3409,7 +3412,7 @@
     <row r="55" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15"/>
       <c r="B55" s="44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C55" s="45"/>
       <c r="D55" s="45"/>
@@ -3461,59 +3464,59 @@
     <row r="59" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
       <c r="B59" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="30" t="s">
         <v>50</v>
-      </c>
-      <c r="C59" s="30" t="s">
-        <v>51</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F59" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
       <c r="B60" s="30"/>
       <c r="C60" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F60" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
       <c r="B61" s="30"/>
       <c r="C61" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F61" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
       <c r="B62" s="30"/>
       <c r="C62" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3522,10 +3525,10 @@
       <c r="C63" s="30"/>
       <c r="D63" s="30"/>
       <c r="E63" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F63" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3533,10 +3536,10 @@
       <c r="C64" s="30"/>
       <c r="D64" s="30"/>
       <c r="E64" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F64" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3558,17 +3561,17 @@
     <row r="67" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
       <c r="B67" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C67" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F67" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3576,10 +3579,10 @@
       <c r="B68" s="30"/>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F68" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3593,38 +3596,38 @@
     <row r="70" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="30"/>
       <c r="B70" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F70" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="30"/>
       <c r="B71" s="30"/>
       <c r="C71" s="30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F71" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="30"/>
       <c r="B72" s="30"/>
       <c r="C72" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30"/>
@@ -3634,7 +3637,7 @@
       <c r="A73" s="30"/>
       <c r="B73" s="30"/>
       <c r="C73" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30"/>
@@ -3644,7 +3647,7 @@
       <c r="A74" s="30"/>
       <c r="B74" s="30"/>
       <c r="C74" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30"/>
@@ -3661,17 +3664,17 @@
     <row r="76" spans="1:6" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="30"/>
       <c r="B76" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C76" s="30" t="s">
         <v>62</v>
-      </c>
-      <c r="C76" s="30" t="s">
-        <v>63</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F76" s="31" t="s">
         <v>65</v>
-      </c>
-      <c r="F76" s="31" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3680,10 +3683,10 @@
       <c r="C77" s="30"/>
       <c r="D77" s="30"/>
       <c r="E77" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F77" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3691,17 +3694,17 @@
       <c r="B78" s="30"/>
       <c r="D78" s="30"/>
       <c r="E78" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="30"/>
       <c r="B79" s="30"/>
       <c r="C79" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30"/>
@@ -3711,7 +3714,7 @@
       <c r="A80" s="30"/>
       <c r="B80" s="30"/>
       <c r="C80" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30"/>
@@ -3721,7 +3724,7 @@
       <c r="A81" s="30"/>
       <c r="B81" s="30"/>
       <c r="C81" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30"/>
@@ -3743,7 +3746,7 @@
       <c r="D83" s="30"/>
       <c r="E83" s="30"/>
       <c r="F83" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3757,13 +3760,13 @@
     <row r="85" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="30"/>
       <c r="B85" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C85" s="30"/>
       <c r="D85" s="30"/>
       <c r="E85" s="30"/>
       <c r="F85" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3773,7 +3776,7 @@
       <c r="D86" s="30"/>
       <c r="E86" s="30"/>
       <c r="F86" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3786,15 +3789,15 @@
     <row r="88" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="30"/>
       <c r="B88" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C88" s="30"/>
       <c r="D88" s="30"/>
       <c r="E88" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F88" s="31" t="s">
         <v>73</v>
-      </c>
-      <c r="F88" s="31" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3808,22 +3811,22 @@
     <row r="90" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="30"/>
       <c r="B90" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30"/>
       <c r="F90" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="30"/>
       <c r="B91" s="30"/>
       <c r="C91" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D91" s="30"/>
       <c r="E91" s="30"/>
@@ -3840,15 +3843,15 @@
     <row r="93" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="30"/>
       <c r="B93" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C93" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D93" s="30"/>
       <c r="E93" s="30"/>
       <c r="F93" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3862,20 +3865,16 @@
     <row r="95" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="30"/>
       <c r="B95" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C95" s="30"/>
       <c r="D95" s="30"/>
       <c r="E95" s="30"/>
       <c r="F95" s="43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="102" spans="6:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F102" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>

</xml_diff>